<commit_message>
tested the connection with static IP
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan_20200804_chiebao.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan_20200804_chiebao.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="814" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="814" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_His." sheetId="3" r:id="rId1"/>
@@ -30,11 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Revision_His.!$A$1:$F$337</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -800,7 +796,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="273">
   <si>
     <t>Test ID</t>
   </si>
@@ -1990,6 +1986,14 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>Not able to do that couse the AP(smartphone) can't
+hide the ssid
+retry in HQ with the D-Link modem, OK.</t>
+  </si>
+  <si>
+    <t>fixed a bug (resolved from version 84)</t>
   </si>
 </sst>
 </file>
@@ -2812,9 +2816,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -6582,7 +6583,7 @@
     </row>
     <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
-        <f t="shared" ref="A3:A4" si="0">A2+1</f>
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -6600,7 +6601,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
-        <f t="shared" si="0"/>
+        <f>A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
@@ -6621,7 +6622,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
-        <f t="shared" ref="A5:A32" si="1">A4+1</f>
+        <f t="shared" ref="A5:A32" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="23"/>
@@ -6630,7 +6631,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="24"/>
@@ -6639,7 +6640,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="23"/>
@@ -6648,7 +6649,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="23"/>
@@ -6657,7 +6658,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="23"/>
@@ -6666,7 +6667,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="23"/>
@@ -6675,7 +6676,7 @@
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="23"/>
@@ -6685,7 +6686,7 @@
     </row>
     <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="23"/>
@@ -6696,7 +6697,7 @@
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="23"/>
@@ -6706,7 +6707,7 @@
     </row>
     <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="23"/>
@@ -6716,7 +6717,7 @@
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="23"/>
@@ -6727,7 +6728,7 @@
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="23"/>
@@ -6737,7 +6738,7 @@
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="23"/>
@@ -6747,7 +6748,7 @@
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="25"/>
@@ -6757,7 +6758,7 @@
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="23"/>
@@ -6767,7 +6768,7 @@
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="23"/>
@@ -6777,7 +6778,7 @@
     </row>
     <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="25"/>
@@ -6787,7 +6788,7 @@
     </row>
     <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="23"/>
@@ -6797,7 +6798,7 @@
     </row>
     <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="24"/>
@@ -6807,7 +6808,7 @@
     </row>
     <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="23"/>
@@ -6817,7 +6818,7 @@
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="23"/>
@@ -6828,7 +6829,7 @@
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="23"/>
@@ -6838,7 +6839,7 @@
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="23"/>
@@ -6848,7 +6849,7 @@
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="23"/>
@@ -6858,7 +6859,7 @@
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="23"/>
@@ -6868,7 +6869,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="24"/>
@@ -6877,7 +6878,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="26"/>
@@ -6887,7 +6888,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="26"/>
@@ -6955,8 +6956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7171,11 +7172,14 @@
       <c r="D11" s="16" t="s">
         <v>144</v>
       </c>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7189,8 +7193,11 @@
       <c r="D12" s="16" t="s">
         <v>202</v>
       </c>
+      <c r="E12" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -7206,6 +7213,12 @@
       </c>
       <c r="D13" s="16" t="s">
         <v>107</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -7357,7 +7370,7 @@
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
-        <f t="shared" ref="A25:A26" si="1">A24+1</f>
+        <f>A24+1</f>
         <v>24</v>
       </c>
       <c r="B25" s="23"/>
@@ -7367,7 +7380,7 @@
     </row>
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
-        <f t="shared" si="1"/>
+        <f>A25+1</f>
         <v>25</v>
       </c>
       <c r="B26" s="25"/>
@@ -7377,7 +7390,7 @@
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
-        <f t="shared" ref="A27:A41" si="2">A26+1</f>
+        <f t="shared" ref="A27:A41" si="1">A26+1</f>
         <v>26</v>
       </c>
       <c r="B27" s="23"/>
@@ -7387,7 +7400,7 @@
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="23"/>
@@ -7397,7 +7410,7 @@
     </row>
     <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="25"/>
@@ -7407,7 +7420,7 @@
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" s="23"/>
@@ -7417,7 +7430,7 @@
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="24"/>
@@ -7427,7 +7440,7 @@
     </row>
     <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" s="23"/>
@@ -7437,7 +7450,7 @@
     </row>
     <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="23"/>
@@ -7448,7 +7461,7 @@
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="23"/>
@@ -7458,7 +7471,7 @@
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="23"/>
@@ -7468,7 +7481,7 @@
     </row>
     <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="23"/>
@@ -7478,7 +7491,7 @@
     </row>
     <row r="37" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="23"/>
@@ -7488,7 +7501,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="24"/>
@@ -7497,7 +7510,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="26"/>
@@ -7507,7 +7520,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="26"/>
@@ -7517,7 +7530,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="23"/>
@@ -8939,7 +8952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>